<commit_message>
Fix bug with missing fallback header and add tests
</commit_message>
<xml_diff>
--- a/test/external-choices.xlsx
+++ b/test/external-choices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanokwa/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanokwa/Documents/Work/Nafundi/Code/yanokwa/pyxform-http/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DD4CFE-F903-A84F-B4BC-77C2F3448C1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F24A1B-5DA7-4743-BD2D-578E0F8FC531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="560" windowWidth="30240" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="560" windowWidth="30240" windowHeight="20020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -3201,7 +3201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
@@ -3240,7 +3240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -3350,7 +3350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>

</xml_diff>